<commit_message>
revise email, application form link and add jobs
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chunyu/Desktop/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chunyu/Desktop/NYCU/2025_TLM_intern/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF9FC07-C24B-AE40-99FB-6ABF25D0D3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61417142-20E1-3A46-A9D1-9E1F74F53AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="25600" windowHeight="15960" xr2:uid="{14D27C65-5EEF-7548-87BB-63F6751C9AE7}"/>
+    <workbookView xWindow="3840" yWindow="680" windowWidth="21760" windowHeight="15960" xr2:uid="{14D27C65-5EEF-7548-87BB-63F6751C9AE7}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="142">
   <si>
     <t>Company</t>
   </si>
@@ -444,6 +444,21 @@
   </si>
   <si>
     <t>https://www.104.com.tw/job/8nwl7?jobsource=index_s_ac</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1O2YeyP1td0ciqUunYCTD48k7vSYGG-XH?dmr=1&amp;ec=wgc-drive-globalnav-goto</t>
+  </si>
+  <si>
+    <t>桃園機場暑期實習</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>桃園</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>大三以上</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1418,11 +1433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE59B568-12D8-C84B-8A47-1A85FB29558E}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2102,6 +2117,26 @@
         <v>137</v>
       </c>
     </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45785</v>
+      </c>
+      <c r="D38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>